<commit_message>
added final jupyter notebook
</commit_message>
<xml_diff>
--- a/hw2/proshares_analysis_data.xlsx
+++ b/hw2/proshares_analysis_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliottgordon/Documents/UChicago/Summer 2025/FINM 25000/finm-25000-a4-repository/hw2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B5A763-4DDD-6947-86F6-FDDC49364EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CE371A-1AC7-5B4D-A30C-34C27C328060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15240" yWindow="780" windowWidth="18960" windowHeight="20780" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="53120" yWindow="-9000" windowWidth="18960" windowHeight="20780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="descriptions" sheetId="1" r:id="rId1"/>
@@ -123,7 +123,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -180,7 +180,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -487,7 +487,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -628,7 +630,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E155"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3278,7 +3282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -6864,6 +6868,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">

</xml_diff>